<commit_message>
Add two more runs and test result file
</commit_message>
<xml_diff>
--- a/migration/ArtifactServicesStress/Runs.xlsx
+++ b/migration/ArtifactServicesStress/Runs.xlsx
@@ -29,7 +29,152 @@
     <author>John Erickson</author>
   </authors>
   <commentList>
-    <comment ref="B8" authorId="0" shapeId="0">
+    <comment ref="D7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>John Erickson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+   Test method Microsoft.VisualStudio.Services.BlobStore.Server.L0.Tests.LiveAzureBlobBlobStoreServiceTestsBug0.RacePutAndRemoveRef threw exception:
+Microsoft.VisualStudio.Services.BlobStore.Server.PlatformBlobStore+BlobMetadataContentionException: Could not cleanup metadata after 100 attempts.
+Stack Trace:
+    at Microsoft.VisualStudio.Services.BlobStore.Server.PlatformBlobStore.&lt;CleanupMetadataAsync&gt;d__46.MoveNext() in D:\src\Artifact2\src\BlobStore\Service\Serve
+r\PlatformBlobStore.cs:line 823
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.ConfiguredTaskAwaitable`1.ConfiguredTaskAwaiter.GetResult()
+   at Microsoft.VisualStudio.Services.BlobStore.Server.PlatformBlobStore.&lt;CheckForDeleteAsync&gt;d__45.MoveNext() in D:\src\Artifact2\src\BlobStore\Service\Server\
+PlatformBlobStore.cs:line 771
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.ConfiguredTaskAwaitable.ConfiguredTaskAwaiter.GetResult()
+   at Microsoft.VisualStudio.Services.BlobStore.Server.PlatformBlobStore.&lt;RemoveReferencesAsync&gt;d__44.MoveNext() in D:\src\Artifact2\src\BlobStore\Service\Serve
+r\PlatformBlobStore.cs:line 756
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.ConfiguredTaskAwaitable.ConfiguredTaskAwaiter.GetResult()
+   at Microsoft.VisualStudio.Services.BlobStore.Server.PlatformBlobStore.&lt;&gt;c__DisplayClass23_1.&lt;&lt;RemoveReferences&gt;b__3&gt;d.MoveNext() in D:\src\Artifact2\src\Blob
+Store\Service\Server\PlatformBlobStore.cs:line 193
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.GetResult()
+   at Microsoft.VisualStudio.Services.BlobStore.Common.TaskSafety.SyncResultOnThreadPool(Func`1 taskFunc) in D:\src\Artifact2\src\ArtifactServices\Shared\BlobSt
+ore.Common\TaskExtensions.cs:line 14
+   at Microsoft.VisualStudio.Services.BlobStore.Server.PlatformBlobStore.RemoveReferences(IVssRequestContext requestContext, IDictionary`2 referenceIdsGroupedBy
+BlobIds) in D:\src\Artifact2\src\BlobStore\Service\Server\PlatformBlobStore.cs:line 210
+   at Microsoft.VisualStudio.Services.BlobStore.Server.Common.BlobStoreExtensions.RemoveReference(IBlobStore blobStore, IVssRequestContext requestContext, BlobI
+dentifier blobId, String referenceId) in D:\src\Artifact2\src\BlobStore\ServiceShared\Server.Common\BlobStoreExtensions.cs:line 32
+   at Microsoft.VisualStudio.Services.BlobStore.Server.L0.Tests.BlobStoreServiceTests`1.&lt;&gt;c__DisplayClass24_1.&lt;&lt;RacePutAndRemoveRefIteration&gt;b__3&gt;d.MoveNext() i
+n D:\src\Artifact2\src\BlobStore\Service\Server.L0.Tests\BlobStoreServiceTests.cs:line 651
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.GetResult()
+   at Microsoft.VisualStudio.Services.BlobStore.Server.L0.Tests.BlobStoreServiceTests`1.&lt;RacePutAndRemoveRefIteration&gt;d__24.MoveNext() in D:\src\Artifact2\src\B
+lobStore\Service\Server.L0.Tests\BlobStoreServiceTests.cs:line 660
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.ConfiguredTaskAwaitable.ConfiguredTaskAwaiter.GetResult()
+   at Microsoft.VisualStudio.Services.BlobStore.Server.L0.Tests.BlobStoreServiceTests`1.&lt;RacePutAndRemoveRef&gt;d__13.MoveNext() in D:\src\Artifact2\src\BlobStore\
+Service\Server.L0.Tests\BlobStoreServiceTests.cs:line 486
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.GetResult()</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>John Erickson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Test Name: RacePutAndRemoveRef
+Test FullName: Microsoft.VisualStudio.Services.BlobStore.Server.L0.Tests.LiveAzureBlobBlobStoreServiceTestsBug2.RacePutAndRemoveRef
+Test Source: D:\src\Artifact2\src\BlobStore\Service\Server.L0.Tests\BlobStoreServiceTests.cs : line 481
+Test Outcome: Failed
+Test Duration: 0:12:43.9910594
+Result StackTrace: 
+at Microsoft.VisualStudio.Services.BlobStore.Server.PlatformBlobStore.&lt;CleanupMetadataAsync&gt;d__46.MoveNext() in D:\src\Artifact2\src\BlobStore\Service\Server\PlatformBlobStore.cs:line 823
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.ConfiguredTaskAwaitable`1.ConfiguredTaskAwaiter.GetResult()
+   at Microsoft.VisualStudio.Services.BlobStore.Server.PlatformBlobStore.&lt;CheckForDeleteAsync&gt;d__45.MoveNext() in D:\src\Artifact2\src\BlobStore\Service\Server\PlatformBlobStore.cs:line 771
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.ConfiguredTaskAwaitable.ConfiguredTaskAwaiter.GetResult()
+   at Microsoft.VisualStudio.Services.BlobStore.Server.PlatformBlobStore.&lt;RemoveReferencesAsync&gt;d__44.MoveNext() in D:\src\Artifact2\src\BlobStore\Service\Server\PlatformBlobStore.cs:line 756
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.ConfiguredTaskAwaitable.ConfiguredTaskAwaiter.GetResult()
+   at Microsoft.VisualStudio.Services.BlobStore.Server.PlatformBlobStore.&lt;&gt;c__DisplayClass23_1.&lt;&lt;RemoveReferences&gt;b__3&gt;d.MoveNext() in D:\src\Artifact2\src\BlobStore\Service\Server\PlatformBlobStore.cs:line 193
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.GetResult()
+   at Microsoft.VisualStudio.Services.BlobStore.Common.TaskSafety.SyncResultOnThreadPool(Func`1 taskFunc) in D:\src\Artifact2\src\ArtifactServices\Shared\BlobStore.Common\TaskExtensions.cs:line 14
+   at Microsoft.VisualStudio.Services.BlobStore.Server.PlatformBlobStore.RemoveReferences(IVssRequestContext requestContext, IDictionary`2 referenceIdsGroupedByBlobIds) in D:\src\Artifact2\src\BlobStore\Service\Server\PlatformBlobStore.cs:line 210
+   at Microsoft.VisualStudio.Services.BlobStore.Server.Common.BlobStoreExtensions.RemoveReference(IBlobStore blobStore, IVssRequestContext requestContext, BlobIdentifier blobId, String referenceId) in D:\src\Artifact2\src\BlobStore\ServiceShared\Server.Common\BlobStoreExtensions.cs:line 32
+   at Microsoft.VisualStudio.Services.BlobStore.Server.L0.Tests.BlobStoreServiceTests`1.&lt;&gt;c__DisplayClass24_1.&lt;&lt;RacePutAndRemoveRefIteration&gt;b__3&gt;d.MoveNext() in D:\src\Artifact2\src\BlobStore\Service\Server.L0.Tests\BlobStoreServiceTests.cs:line 651
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.GetResult()
+   at Microsoft.VisualStudio.Services.BlobStore.Server.L0.Tests.BlobStoreServiceTests`1.&lt;RacePutAndRemoveRefIteration&gt;d__24.MoveNext() in D:\src\Artifact2\src\BlobStore\Service\Server.L0.Tests\BlobStoreServiceTests.cs:line 660
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.ConfiguredTaskAwaitable.ConfiguredTaskAwaiter.GetResult()
+   at Microsoft.VisualStudio.Services.BlobStore.Server.L0.Tests.BlobStoreServiceTests`1.&lt;RacePutAndRemoveRef&gt;d__13.MoveNext() in D:\src\Artifact2\src\BlobStore\Service\Server.L0.Tests\BlobStoreServiceTests.cs:line 486
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.GetResult()
+Result Message: 
+Test method Microsoft.VisualStudio.Services.BlobStore.Server.L0.Tests.LiveAzureBlobBlobStoreServiceTestsBug2.RacePutAndRemoveRef threw exception: 
+Microsoft.VisualStudio.Services.BlobStore.Server.PlatformBlobStore+BlobMetadataContentionException: Could not cleanup metadata after 100 attempts.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -115,12 +260,58 @@
         </r>
       </text>
     </comment>
+    <comment ref="C18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>John Erickson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Test Name: RacePutAndRemoveRef
+Test FullName: Microsoft.VisualStudio.Services.BlobStore.Server.L0.Tests.LiveAzureBlobBlobStoreServiceTestsBug11.RacePutAndRemoveRef
+Test Source: D:\src\Artifact2\src\BlobStore\Service\Server.L0.Tests\BlobStoreServiceTests.cs : line 481
+Test Outcome: Failed
+Test Duration: 0:16:30.361526
+Result StackTrace: 
+at Microsoft.VisualStudio.Services.BlobStore.Server.L0.Tests.BlobStoreServiceTests`1.&lt;&gt;c__DisplayClass24_1.&lt;&lt;RacePutAndRemoveRefIteration&gt;b__3&gt;d.MoveNext() in D:\src\Artifact2\src\BlobStore\Service\Server.L0.Tests\BlobStoreServiceTests.cs:line 646
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.GetResult()
+   at Microsoft.VisualStudio.Services.BlobStore.Server.L0.Tests.BlobStoreServiceTests`1.&lt;RacePutAndRemoveRefIteration&gt;d__24.MoveNext() in D:\src\Artifact2\src\BlobStore\Service\Server.L0.Tests\BlobStoreServiceTests.cs:line 660
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.ConfiguredTaskAwaitable.ConfiguredTaskAwaiter.GetResult()
+   at Microsoft.VisualStudio.Services.BlobStore.Server.L0.Tests.BlobStoreServiceTests`1.&lt;RacePutAndRemoveRef&gt;d__13.MoveNext() in D:\src\Artifact2\src\BlobStore\Service\Server.L0.Tests\BlobStoreServiceTests.cs:line 486
+--- End of stack trace from previous location where exception was thrown ---
+   at System.Runtime.CompilerServices.TaskAwaiter.ThrowForNonSuccess(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.HandleNonSuccessAndDebuggerNotification(Task task)
+   at System.Runtime.CompilerServices.TaskAwaiter.GetResult()
+Result Message: Assert.IsNotNull failed. Microsoft.VisualStudio.Services.BlobStore.Server.L0.Tests.LiveAzureBlobBlobStoreServiceTestsBug11 TryRefSuccess:75 TryRefFail:15 Refs:1
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
   <si>
     <t>Iterations</t>
   </si>
@@ -177,6 +368,18 @@
   </si>
   <si>
     <t>Run 2</t>
+  </si>
+  <si>
+    <t>Run 3</t>
+  </si>
+  <si>
+    <t>TestFile</t>
+  </si>
+  <si>
+    <t>jerick_JERICK-DEBUG 2015-09-18 23_41_53.trx</t>
+  </si>
+  <si>
+    <t>Bugless</t>
   </si>
 </sst>
 </file>
@@ -507,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,15 +721,18 @@
     <col min="1" max="1" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -536,8 +742,11 @@
       <c r="C2">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -547,8 +756,11 @@
       <c r="C3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -556,102 +768,199 @@
         <v>12</v>
       </c>
       <c r="C4">
+        <v>24</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="D18" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>